<commit_message>
Update Descrição dos Casos de Uso.xlsx
</commit_message>
<xml_diff>
--- a/files/Casos de Uso/Descrição dos Casos de Uso.xlsx
+++ b/files/Casos de Uso/Descrição dos Casos de Uso.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="-15855" windowWidth="23490" windowHeight="13560" tabRatio="736"/>
+    <workbookView xWindow="2865" yWindow="-15855" windowWidth="23490" windowHeight="13560" tabRatio="736" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CSU01" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="209">
   <si>
     <t>Nome do Caso de Uso</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Serão exibidos os dados das categorias de evento</t>
   </si>
   <si>
-    <t>1 Seleciona a opção "Listar"</t>
-  </si>
-  <si>
     <t>Permite exibir eventos</t>
   </si>
   <si>
@@ -674,9 +671,6 @@
   </si>
   <si>
     <t>9 Exibe os ingressos</t>
-  </si>
-  <si>
-    <t>2 Exibe os dados solicitados</t>
   </si>
   <si>
     <t>5 Exclui a organizadora</t>
@@ -1114,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1218,16 +1212,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1251,17 +1236,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1550,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1600,10 +1603,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1640,14 +1643,14 @@
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -1660,14 +1663,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="38"/>
+      <c r="A16" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -1680,7 +1683,7 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1728,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1744,14 +1747,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1763,39 +1766,39 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -1808,14 +1811,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -1828,14 +1831,14 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="48"/>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -1848,7 +1851,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1900,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1913,14 +1916,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1932,20 +1935,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="40"/>
+      <c r="A9" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="37"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1991,7 +1994,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2007,58 +2010,58 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -2071,14 +2074,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -2091,14 +2094,14 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="48"/>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -2111,7 +2114,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2160,7 +2163,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2176,14 +2179,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
@@ -2195,13 +2198,13 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="28"/>
     </row>
@@ -2214,7 +2217,7 @@
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2260,7 +2263,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2276,14 +2279,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -2295,39 +2298,39 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -2340,14 +2343,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -2360,14 +2363,14 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="48"/>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -2380,7 +2383,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2432,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2445,14 +2448,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -2464,45 +2467,45 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="48"/>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -2515,14 +2518,14 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="48"/>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -2535,14 +2538,14 @@
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="48"/>
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -2555,7 +2558,7 @@
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2604,7 +2607,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2620,14 +2623,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -2639,45 +2642,45 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="48"/>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -2690,7 +2693,7 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2737,7 +2740,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2753,14 +2756,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -2772,39 +2775,39 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -2817,14 +2820,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -2837,14 +2840,14 @@
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="48"/>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -2857,7 +2860,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2906,7 +2909,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2922,14 +2925,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -2941,45 +2944,45 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="48"/>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -2992,14 +2995,14 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="48"/>
     </row>
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -3012,14 +3015,14 @@
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="48"/>
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -3032,7 +3035,7 @@
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3081,7 +3084,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3097,14 +3100,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -3116,45 +3119,45 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="48"/>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -3167,7 +3170,7 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3234,10 +3237,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -3249,14 +3252,14 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3302,7 +3305,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3310,14 +3313,14 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="46"/>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -3329,39 +3332,39 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B7" s="13"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="48"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -3374,14 +3377,14 @@
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="48"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -3394,14 +3397,14 @@
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="48"/>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
@@ -3414,7 +3417,7 @@
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3463,7 +3466,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3479,58 +3482,58 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -3543,14 +3546,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -3563,14 +3566,14 @@
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="48"/>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -3583,7 +3586,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3632,7 +3635,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3648,64 +3651,64 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="49" t="s">
-        <v>207</v>
+      <c r="A12" s="43"/>
+      <c r="B12" s="44" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25"/>
       <c r="B13" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="47"/>
+      <c r="A14" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="50"/>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -3718,14 +3721,14 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="B17" s="38"/>
+      <c r="A17" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="48"/>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -3738,7 +3741,7 @@
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3786,7 +3789,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3802,14 +3805,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -3821,39 +3824,39 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -3866,14 +3869,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -3886,7 +3889,7 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3934,7 +3937,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3950,14 +3953,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -3969,39 +3972,39 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -4014,14 +4017,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -4034,14 +4037,14 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="38"/>
+      <c r="A19" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="48"/>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -4054,7 +4057,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4103,7 +4106,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4119,14 +4122,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -4138,39 +4141,39 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="38"/>
+      <c r="A13" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -4183,7 +4186,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4230,7 +4233,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4246,14 +4249,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -4265,45 +4268,45 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="48"/>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -4316,14 +4319,14 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="48"/>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -4336,14 +4339,14 @@
     <row r="19" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" s="38"/>
+      <c r="A20" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="48"/>
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -4356,7 +4359,7 @@
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4405,7 +4408,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4421,14 +4424,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -4440,26 +4443,26 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="B8" s="41"/>
+        <v>173</v>
+      </c>
+      <c r="B8" s="38"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4476,7 +4479,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4505,7 +4508,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4521,14 +4524,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -4540,51 +4543,51 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B13" s="13"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="48"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -4597,14 +4600,14 @@
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="48"/>
     </row>
     <row r="19" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
@@ -4617,14 +4620,14 @@
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" s="38"/>
+      <c r="A21" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="48"/>
     </row>
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
@@ -4637,7 +4640,7 @@
     <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4686,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4702,14 +4705,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -4721,45 +4724,45 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="48"/>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -4772,7 +4775,7 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4819,7 +4822,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4835,14 +4838,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
@@ -4854,26 +4857,26 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
-      <c r="B9" s="45" t="s">
-        <v>135</v>
+      <c r="B9" s="42" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4919,7 +4922,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4927,14 +4930,14 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="46"/>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -4946,39 +4949,39 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B7" s="13"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="48"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -4991,14 +4994,14 @@
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="48"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -5011,14 +5014,14 @@
     <row r="17" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="48"/>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
@@ -5031,7 +5034,7 @@
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -5080,7 +5083,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5096,58 +5099,58 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -5160,14 +5163,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -5180,14 +5183,14 @@
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="48"/>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -5200,7 +5203,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -5249,7 +5252,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5265,57 +5268,57 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="49" t="s">
-        <v>195</v>
+      <c r="A12" s="43"/>
+      <c r="B12" s="44" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25"/>
       <c r="B13" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -5361,7 +5364,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5377,82 +5380,82 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B12" s="28"/>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13" s="28"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
-      <c r="B14" s="45" t="s">
-        <v>203</v>
+      <c r="B14" s="42" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
-      <c r="B15" s="45" t="s">
-        <v>204</v>
+      <c r="B15" s="42" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25"/>
       <c r="B16" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -5465,14 +5468,14 @@
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="48"/>
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -5485,7 +5488,7 @@
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -5501,10 +5504,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5533,7 +5536,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5549,34 +5552,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="B8" s="13"/>
     </row>
-    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21" t="s">
-        <v>206</v>
-      </c>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5621,7 +5630,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5637,14 +5646,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -5656,20 +5665,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="40"/>
+      <c r="A9" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="37"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -5715,7 +5724,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5731,14 +5740,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -5750,39 +5759,39 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="44"/>
+        <v>139</v>
+      </c>
+      <c r="B9" s="41"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -5795,14 +5804,14 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="48"/>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -5815,7 +5824,7 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -5863,7 +5872,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5879,14 +5888,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
@@ -5898,20 +5907,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -5957,7 +5966,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5973,14 +5982,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -5992,20 +6001,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="40"/>
+      <c r="A9" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="37"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -6051,7 +6060,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -6067,14 +6076,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -6086,20 +6095,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sincronizando os dados entre documentos
</commit_message>
<xml_diff>
--- a/files/Casos de Uso/Descrição dos Casos de Uso.xlsx
+++ b/files/Casos de Uso/Descrição dos Casos de Uso.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="-15855" windowWidth="23490" windowHeight="13560" tabRatio="736" activeTab="3"/>
+    <workbookView xWindow="2865" yWindow="-15855" windowWidth="23490" windowHeight="13560" tabRatio="736" firstSheet="10" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="CSU01" sheetId="2" r:id="rId1"/>
@@ -25,23 +25,23 @@
     <sheet name="CSU11" sheetId="16" r:id="rId11"/>
     <sheet name="CSU12" sheetId="17" r:id="rId12"/>
     <sheet name="CSU13" sheetId="18" r:id="rId13"/>
-    <sheet name="CSU17" sheetId="32" r:id="rId14"/>
-    <sheet name="CSU18" sheetId="33" r:id="rId15"/>
-    <sheet name="CSU19" sheetId="34" r:id="rId16"/>
-    <sheet name="CSU20" sheetId="35" r:id="rId17"/>
-    <sheet name="CSU21" sheetId="36" r:id="rId18"/>
-    <sheet name="CSU22" sheetId="37" r:id="rId19"/>
-    <sheet name="CSU23" sheetId="38" r:id="rId20"/>
-    <sheet name="CSU24" sheetId="39" r:id="rId21"/>
-    <sheet name="CSU25" sheetId="40" r:id="rId22"/>
-    <sheet name="CSU26" sheetId="41" r:id="rId23"/>
-    <sheet name="CSU27" sheetId="42" r:id="rId24"/>
-    <sheet name="CSU28" sheetId="43" r:id="rId25"/>
-    <sheet name="CSU29" sheetId="44" r:id="rId26"/>
-    <sheet name="CSU30" sheetId="45" r:id="rId27"/>
-    <sheet name="CSU31" sheetId="48" r:id="rId28"/>
-    <sheet name="CSU32" sheetId="46" r:id="rId29"/>
-    <sheet name="CSU33" sheetId="47" r:id="rId30"/>
+    <sheet name="CSU14" sheetId="32" r:id="rId14"/>
+    <sheet name="CSU15" sheetId="33" r:id="rId15"/>
+    <sheet name="CSU16" sheetId="34" r:id="rId16"/>
+    <sheet name="CSU17" sheetId="35" r:id="rId17"/>
+    <sheet name="CSU18" sheetId="36" r:id="rId18"/>
+    <sheet name="CSU19" sheetId="37" r:id="rId19"/>
+    <sheet name="CSU20" sheetId="38" r:id="rId20"/>
+    <sheet name="CSU21" sheetId="39" r:id="rId21"/>
+    <sheet name="CSU22" sheetId="40" r:id="rId22"/>
+    <sheet name="CSU23" sheetId="41" r:id="rId23"/>
+    <sheet name="CSU24" sheetId="42" r:id="rId24"/>
+    <sheet name="CSU25" sheetId="43" r:id="rId25"/>
+    <sheet name="CSU26" sheetId="44" r:id="rId26"/>
+    <sheet name="CSU27" sheetId="45" r:id="rId27"/>
+    <sheet name="CSU28" sheetId="48" r:id="rId28"/>
+    <sheet name="CSU29" sheetId="46" r:id="rId29"/>
+    <sheet name="CSU30" sheetId="47" r:id="rId30"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -133,60 +133,21 @@
     <t>CSU-09: Exibir Pedido</t>
   </si>
   <si>
-    <t>CSU-17: Cadastrar Categoria de Evento</t>
-  </si>
-  <si>
-    <t>CSU-18: Editar Categoria de Evento</t>
-  </si>
-  <si>
-    <t>CSU-19: Excluir Categoria de Evento</t>
-  </si>
-  <si>
-    <t>CSU-20: Cadastrar Organizadora</t>
-  </si>
-  <si>
     <t>Organizadora</t>
   </si>
   <si>
-    <t>CSU-21: Editar Organizadora</t>
-  </si>
-  <si>
-    <t>CSU-22: Excluir Organizadora</t>
-  </si>
-  <si>
-    <t>CSU-23: Cadastrar Evento</t>
-  </si>
-  <si>
-    <t>CSU-24: Editar Evento</t>
-  </si>
-  <si>
-    <t>CSU-25: Excluir Evento</t>
-  </si>
-  <si>
     <t>Fluxo Alternativo I - Existem dados dependentes desse cadastro no sistema</t>
   </si>
   <si>
     <t>Comprador</t>
   </si>
   <si>
-    <t>CSU-30: Cadastrar Comprador</t>
-  </si>
-  <si>
-    <t>CSU-31: Editar Comprador</t>
-  </si>
-  <si>
-    <t>CSU-33: Efetuar Pedido</t>
-  </si>
-  <si>
     <t>Fluxo Alternativo I - Valor é superior ao da carteira</t>
   </si>
   <si>
     <t>CSU-06: Efetuar Saque</t>
   </si>
   <si>
-    <t>CSU-32: Excluir Comprador</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -616,30 +577,18 @@
     <t>Permite excluir uma categoria de eventos</t>
   </si>
   <si>
-    <t>CSU-26: Cadastrar Tipo de Ingresso</t>
-  </si>
-  <si>
     <t>3 Clica em "Cadastrar Tipo de Ingresso"</t>
   </si>
   <si>
-    <t>CSU-27: Exibir Tipo de Ingresso</t>
-  </si>
-  <si>
     <t>3 Clica em "Tipos de Ingressos"</t>
   </si>
   <si>
     <t>4 Exibe os tipos de ingressos em um evento</t>
   </si>
   <si>
-    <t>CSU-28: Editar Tipo de Ingresso</t>
-  </si>
-  <si>
     <t>3 Clica em "Tipo de Ingressos"</t>
   </si>
   <si>
-    <t>CSU-29: Excluir Tipo de Ingresso</t>
-  </si>
-  <si>
     <t>3 Clica em "Tipos de Ingresso"</t>
   </si>
   <si>
@@ -656,6 +605,57 @@
   </si>
   <si>
     <t>CSU-04: Editar Conta ADM</t>
+  </si>
+  <si>
+    <t>CSU-14: Cadastrar Categoria de Evento</t>
+  </si>
+  <si>
+    <t>CSU-15: Editar Categoria de Evento</t>
+  </si>
+  <si>
+    <t>CSU-16: Excluir Categoria de Evento</t>
+  </si>
+  <si>
+    <t>CSU-17: Cadastrar Organizadora</t>
+  </si>
+  <si>
+    <t>CSU-18: Editar Organizadora</t>
+  </si>
+  <si>
+    <t>CSU-19: Excluir Organizadora</t>
+  </si>
+  <si>
+    <t>CSU-20: Cadastrar Evento</t>
+  </si>
+  <si>
+    <t>CSU-21: Editar Evento</t>
+  </si>
+  <si>
+    <t>CSU-22: Excluir Evento</t>
+  </si>
+  <si>
+    <t>CSU-23: Cadastrar Tipo de Ingresso</t>
+  </si>
+  <si>
+    <t>CSU-24: Exibir Tipo de Ingresso</t>
+  </si>
+  <si>
+    <t>CSU-25: Editar Tipo de Ingresso</t>
+  </si>
+  <si>
+    <t>CSU-26: Excluir Tipo de Ingresso</t>
+  </si>
+  <si>
+    <t>CSU-27: Cadastrar Comprador</t>
+  </si>
+  <si>
+    <t>CSU-28: Editar Comprador</t>
+  </si>
+  <si>
+    <t>CSU-29: Excluir Comprador</t>
+  </si>
+  <si>
+    <t>CSU-30: Efetuar Pedido</t>
   </si>
 </sst>
 </file>
@@ -1550,7 +1550,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1566,7 +1566,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1585,32 +1585,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1630,12 +1630,12 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="47" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B16" s="48"/>
     </row>
@@ -1650,7 +1650,7 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1698,7 +1698,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1706,7 +1706,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1714,7 +1714,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1733,32 +1733,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1778,7 +1778,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1798,12 +1798,12 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B19" s="48"/>
     </row>
@@ -1818,7 +1818,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1867,7 +1867,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1875,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1883,7 +1883,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1902,20 +1902,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="36"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1961,7 +1961,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1969,7 +1969,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1977,7 +1977,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1996,32 +1996,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="29" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2041,7 +2041,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2061,12 +2061,12 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B19" s="48"/>
     </row>
@@ -2081,7 +2081,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2130,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2138,7 +2138,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2146,7 +2146,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2165,13 +2165,13 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B9" s="28"/>
     </row>
@@ -2184,7 +2184,7 @@
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="29" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2201,7 +2201,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>26</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2238,7 +2238,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2246,7 +2246,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2265,32 +2265,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2310,7 +2310,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2330,12 +2330,12 @@
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B19" s="48"/>
     </row>
@@ -2350,7 +2350,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2370,7 +2370,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,7 +2383,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>27</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2399,7 +2399,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2415,7 +2415,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2434,38 +2434,38 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2485,7 +2485,7 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2505,12 +2505,12 @@
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B20" s="48"/>
     </row>
@@ -2525,7 +2525,7 @@
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2545,7 +2545,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2574,7 +2574,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2590,7 +2590,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2609,43 +2609,43 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B14" s="48"/>
     </row>
@@ -2660,7 +2660,7 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2678,7 +2678,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2691,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>29</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2699,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2715,7 +2715,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2734,32 +2734,32 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="B7" s="13"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2779,7 +2779,7 @@
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2799,12 +2799,12 @@
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B18" s="48"/>
     </row>
@@ -2819,7 +2819,7 @@
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2839,7 +2839,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2852,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>31</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2876,7 +2876,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2884,7 +2884,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2903,32 +2903,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="29" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2948,7 +2948,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2968,12 +2968,12 @@
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B19" s="48"/>
     </row>
@@ -2988,7 +2988,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3008,7 +3008,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3021,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>32</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3029,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3045,7 +3045,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3053,7 +3053,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3072,43 +3072,43 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25"/>
       <c r="B13" s="29" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B14" s="50"/>
     </row>
@@ -3123,12 +3123,12 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="47" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B17" s="48"/>
     </row>
@@ -3143,7 +3143,7 @@
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3183,7 +3183,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3191,7 +3191,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3199,7 +3199,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3207,7 +3207,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3226,14 +3226,14 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="21" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3250,7 +3250,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3295,7 +3295,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3314,32 +3314,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3359,7 +3359,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3379,7 +3379,7 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3398,7 +3398,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,7 +3411,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3419,7 +3419,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3427,7 +3427,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3443,7 +3443,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3462,32 +3462,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3507,7 +3507,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3527,12 +3527,12 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B19" s="48"/>
     </row>
@@ -3547,7 +3547,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3567,7 +3567,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3580,7 +3580,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>35</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3588,7 +3588,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3604,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3612,7 +3612,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3631,37 +3631,37 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B13" s="48"/>
     </row>
@@ -3676,7 +3676,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3694,7 +3694,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3707,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3715,7 +3715,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -3723,7 +3723,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3731,7 +3731,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3739,7 +3739,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3758,38 +3758,38 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3809,7 +3809,7 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3829,12 +3829,12 @@
     <row r="19" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B20" s="48"/>
     </row>
@@ -3849,7 +3849,7 @@
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3869,7 +3869,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,7 +3882,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3890,7 +3890,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -3898,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3906,7 +3906,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3914,7 +3914,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3933,26 +3933,26 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B8" s="37"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="21" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3969,7 +3969,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -3998,7 +3998,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4006,7 +4006,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4014,7 +4014,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4033,44 +4033,44 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B13" s="13"/>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4090,7 +4090,7 @@
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4110,12 +4110,12 @@
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="47" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B21" s="48"/>
     </row>
@@ -4130,7 +4130,7 @@
     <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4150,7 +4150,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4163,7 +4163,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4171,7 +4171,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -4179,7 +4179,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4187,7 +4187,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4195,7 +4195,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4214,43 +4214,43 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B14" s="48"/>
     </row>
@@ -4265,7 +4265,7 @@
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4283,7 +4283,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4296,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4304,7 +4304,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4312,7 +4312,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4320,7 +4320,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4339,32 +4339,32 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="B7" s="13"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4384,7 +4384,7 @@
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4404,12 +4404,12 @@
     <row r="17" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B18" s="48"/>
     </row>
@@ -4424,7 +4424,7 @@
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -4444,7 +4444,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4457,7 +4457,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4465,7 +4465,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4473,7 +4473,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4481,7 +4481,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4508,32 +4508,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="29" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4553,7 +4553,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4573,12 +4573,12 @@
     <row r="18" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B19" s="48"/>
     </row>
@@ -4593,7 +4593,7 @@
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -4613,7 +4613,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4626,7 +4626,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4642,7 +4642,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4650,7 +4650,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4658,7 +4658,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4677,38 +4677,38 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25"/>
       <c r="B13" s="29" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4746,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4754,7 +4754,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4762,7 +4762,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4770,7 +4770,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4789,26 +4789,26 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="41" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="29" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -4824,8 +4824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4838,7 +4838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>40</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4846,7 +4846,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -4854,7 +4854,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4862,7 +4862,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4870,7 +4870,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4889,56 +4889,56 @@
     </row>
     <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B12" s="28"/>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B13" s="28"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="41" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="41" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25"/>
       <c r="B16" s="29" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4958,7 +4958,7 @@
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4978,7 +4978,7 @@
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4996,7 +4996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5010,7 +5010,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5026,7 +5026,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5034,7 +5034,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5042,7 +5042,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5061,32 +5061,32 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5106,7 +5106,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5126,7 +5126,7 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5174,7 +5174,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5182,7 +5182,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5190,7 +5190,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5209,20 +5209,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="36"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -5252,7 +5252,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5268,7 +5268,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5276,7 +5276,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5284,7 +5284,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5303,37 +5303,37 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B9" s="40"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="33" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B13" s="48"/>
     </row>
@@ -5348,7 +5348,7 @@
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5368,7 +5368,7 @@
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5416,7 +5416,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5424,7 +5424,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5432,7 +5432,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5451,20 +5451,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="29" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -5510,7 +5510,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5518,7 +5518,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5526,7 +5526,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5545,20 +5545,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B9" s="36"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -5604,7 +5604,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5620,7 +5620,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5639,20 +5639,20 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="29" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>